<commit_message>
Update universal project tracker
</commit_message>
<xml_diff>
--- a/Project tracker.xlsx
+++ b/Project tracker.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270C1796-008C-4609-A056-CABF440DBF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BDACB8-4CCA-402D-843C-F093367ADDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project tracker" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Category</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Project Task Tracker</t>
   </si>
   <si>
-    <t>Student 1</t>
-  </si>
-  <si>
     <t>Student 2</t>
   </si>
   <si>
@@ -161,6 +158,42 @@
   </si>
   <si>
     <t>Task Description</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Game Logic</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Leaderboard</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Game Functionality</t>
+  </si>
+  <si>
+    <t>Game Functionality Testing</t>
   </si>
 </sst>
 </file>
@@ -624,56 +657,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="3" tint="-0.499984740745262"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="3" tint="-0.499984740745262"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -702,6 +685,31 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -761,6 +769,31 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1231,16 +1264,16 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Estimated start" dataDxfId="14"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Estimated finish" dataDxfId="13"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Estimated work (in hours)" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Estimated duration_x000a_(in days)" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Estimated duration_x000a_(in days)" dataDxfId="11">
       <calculatedColumnFormula>IF(COUNTA('Project tracker'!$E5,'Project tracker'!$F5)&lt;&gt;2,"",DAYS360('Project tracker'!$E5,'Project tracker'!$F5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Actual start" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Actual finish" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Actual work _x000a_(in hours)" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Actual duration (in days)" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Actual start" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Actual finish" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Actual work _x000a_(in hours)" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Actual duration (in days)" dataDxfId="7">
       <calculatedColumnFormula>IF(COUNTA('Project tracker'!$I5,'Project tracker'!$J5)&lt;&gt;2,"",DAYS360('Project tracker'!$I5,'Project tracker'!$J5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Notes" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Custom Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1252,14 +1285,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="CategoryAndEmployeeTable" displayName="CategoryAndEmployeeTable" ref="B4:C10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="CategoryAndEmployeeTable" displayName="CategoryAndEmployeeTable" ref="B4:C10" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="B4:C10" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category Name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Employee Name" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category Name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Employee Name" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Custom Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1504,25 +1537,25 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B16" sqref="B16:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" style="3" customWidth="1"/>
-    <col min="2" max="4" width="18.7265625" style="19" customWidth="1"/>
-    <col min="5" max="6" width="18.7265625" style="20" customWidth="1"/>
-    <col min="7" max="8" width="18.7265625" style="19" customWidth="1"/>
-    <col min="9" max="10" width="16.81640625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="6.69921875" style="3" customWidth="1"/>
+    <col min="2" max="4" width="18.69921875" style="19" customWidth="1"/>
+    <col min="5" max="6" width="18.69921875" style="20" customWidth="1"/>
+    <col min="7" max="8" width="18.69921875" style="19" customWidth="1"/>
+    <col min="9" max="10" width="16.796875" style="20" customWidth="1"/>
     <col min="11" max="12" width="16" style="19" customWidth="1"/>
-    <col min="13" max="13" width="20.36328125" style="19" customWidth="1"/>
-    <col min="14" max="14" width="6.7265625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="4.1796875" style="2" customWidth="1"/>
-    <col min="16" max="40" width="3.26953125" style="2" customWidth="1"/>
-    <col min="41" max="16384" width="9.08984375" style="2"/>
+    <col min="13" max="13" width="20.3984375" style="19" customWidth="1"/>
+    <col min="14" max="14" width="6.69921875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="4.19921875" style="2" customWidth="1"/>
+    <col min="16" max="40" width="3.296875" style="2" customWidth="1"/>
+    <col min="41" max="16384" width="9.09765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1538,7 +1571,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="26" t="s">
         <v>31</v>
@@ -1560,7 +1593,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1576,7 +1609,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="17" t="s">
         <v>21</v>
@@ -1616,95 +1649,91 @@
       </c>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="18" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E5" s="25">
-        <f ca="1">TODAY()-65</f>
-        <v>45485</v>
+        <v>45604</v>
       </c>
       <c r="F5" s="25">
-        <f ca="1">TODAY()-5</f>
-        <v>45545</v>
+        <v>45621</v>
       </c>
       <c r="G5" s="18">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="H5" s="21">
-        <f ca="1">IF(COUNTA('Project tracker'!$E5,'Project tracker'!$F5)&lt;&gt;2,"",DAYS360('Project tracker'!$E5,'Project tracker'!$F5,FALSE))</f>
-        <v>58</v>
+        <f>IF(COUNTA('Project tracker'!$E5,'Project tracker'!$F5)&lt;&gt;2,"",DAYS360('Project tracker'!$E5,'Project tracker'!$F5,FALSE))</f>
+        <v>17</v>
       </c>
       <c r="I5" s="25">
         <f ca="1">TODAY()-65</f>
-        <v>45485</v>
+        <v>45531</v>
       </c>
       <c r="J5" s="25">
         <f ca="1">TODAY()</f>
-        <v>45550</v>
+        <v>45596</v>
       </c>
       <c r="K5" s="18">
         <v>5</v>
       </c>
       <c r="L5" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$I5,'Project tracker'!$J5)&lt;&gt;2,"",DAYS360('Project tracker'!$I5,'Project tracker'!$J5,FALSE))</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M5" s="18"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="25">
+        <v>45619</v>
+      </c>
+      <c r="F6" s="25">
+        <v>45622</v>
+      </c>
+      <c r="G6" s="18">
+        <v>9</v>
+      </c>
+      <c r="H6" s="21">
+        <f>IF(COUNTA('Project tracker'!$E6,'Project tracker'!$F6)&lt;&gt;2,"",DAYS360('Project tracker'!$E6,'Project tracker'!$F6,FALSE))</f>
         <v>3</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="25">
-        <f ca="1">TODAY()-41</f>
-        <v>45509</v>
-      </c>
-      <c r="F6" s="25">
-        <f ca="1">TODAY()-10</f>
-        <v>45540</v>
-      </c>
-      <c r="G6" s="18">
-        <v>4</v>
-      </c>
-      <c r="H6" s="21">
-        <f ca="1">IF(COUNTA('Project tracker'!$E6,'Project tracker'!$F6)&lt;&gt;2,"",DAYS360('Project tracker'!$E6,'Project tracker'!$F6,FALSE))</f>
-        <v>30</v>
       </c>
       <c r="I6" s="25">
         <f ca="1">TODAY()-41</f>
-        <v>45509</v>
+        <v>45555</v>
       </c>
       <c r="J6" s="25">
         <f ca="1">TODAY()-7</f>
-        <v>45543</v>
+        <v>45589</v>
       </c>
       <c r="K6" s="18">
         <v>6</v>
       </c>
       <c r="L6" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$I6,'Project tracker'!$J6)&lt;&gt;2,"",DAYS360('Project tracker'!$I6,'Project tracker'!$J6,FALSE))</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M6" s="18"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="18" t="s">
         <v>24</v>
@@ -1713,42 +1742,42 @@
         <v>2</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="25">
         <f ca="1">TODAY()-100</f>
-        <v>45450</v>
+        <v>45496</v>
       </c>
       <c r="F7" s="25">
         <f ca="1">TODAY()-40</f>
-        <v>45510</v>
+        <v>45556</v>
       </c>
       <c r="G7" s="18">
         <v>5</v>
       </c>
       <c r="H7" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$E7,'Project tracker'!$F7)&lt;&gt;2,"",DAYS360('Project tracker'!$E7,'Project tracker'!$F7,FALSE))</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" s="25">
         <f ca="1">TODAY()-100</f>
-        <v>45450</v>
+        <v>45496</v>
       </c>
       <c r="J7" s="25">
         <f ca="1">TODAY()-27</f>
-        <v>45523</v>
+        <v>45569</v>
       </c>
       <c r="K7" s="18">
         <v>4</v>
       </c>
       <c r="L7" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$I7,'Project tracker'!$J7)&lt;&gt;2,"",DAYS360('Project tracker'!$I7,'Project tracker'!$J7,FALSE))</f>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M7" s="18"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="18" t="s">
         <v>25</v>
@@ -1757,15 +1786,15 @@
         <v>3</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45460</v>
+        <v>45506</v>
       </c>
       <c r="F8" s="25">
         <f ca="1">TODAY()-80</f>
-        <v>45470</v>
+        <v>45516</v>
       </c>
       <c r="G8" s="18">
         <v>6</v>
@@ -1776,11 +1805,11 @@
       </c>
       <c r="I8" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45460</v>
+        <v>45506</v>
       </c>
       <c r="J8" s="25">
         <f ca="1">TODAY()-71</f>
-        <v>45479</v>
+        <v>45525</v>
       </c>
       <c r="K8" s="18">
         <v>1</v>
@@ -1792,7 +1821,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="18" t="s">
         <v>26</v>
@@ -1801,30 +1830,30 @@
         <v>4</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45460</v>
+        <v>45506</v>
       </c>
       <c r="F9" s="25">
         <f ca="1">TODAY()-50</f>
-        <v>45500</v>
+        <v>45546</v>
       </c>
       <c r="G9" s="18">
         <v>4</v>
       </c>
       <c r="H9" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$E9,'Project tracker'!$F9)&lt;&gt;2,"",DAYS360('Project tracker'!$E9,'Project tracker'!$F9,FALSE))</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I9" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45460</v>
+        <v>45506</v>
       </c>
       <c r="J9" s="25">
         <f ca="1">TODAY()-44</f>
-        <v>45506</v>
+        <v>45552</v>
       </c>
       <c r="K9" s="18">
         <v>1</v>
@@ -1836,7 +1865,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="18" t="s">
         <v>27</v>
@@ -1845,15 +1874,15 @@
         <v>5</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="25">
         <f ca="1">TODAY()-60</f>
-        <v>45490</v>
+        <v>45536</v>
       </c>
       <c r="F10" s="25">
         <f ca="1">TODAY()-50</f>
-        <v>45500</v>
+        <v>45546</v>
       </c>
       <c r="G10" s="18">
         <v>5</v>
@@ -1864,23 +1893,23 @@
       </c>
       <c r="I10" s="25">
         <f ca="1">TODAY()-60</f>
-        <v>45490</v>
+        <v>45536</v>
       </c>
       <c r="J10" s="25">
         <f ca="1">TODAY()-45</f>
-        <v>45505</v>
+        <v>45551</v>
       </c>
       <c r="K10" s="18">
         <v>6</v>
       </c>
       <c r="L10" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$I10,'Project tracker'!$J10)&lt;&gt;2,"",DAYS360('Project tracker'!$I10,'Project tracker'!$J10,FALSE))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="18" t="s">
         <v>28</v>
@@ -1889,15 +1918,15 @@
         <v>6</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="25">
         <f ca="1">TODAY()-44</f>
-        <v>45506</v>
+        <v>45552</v>
       </c>
       <c r="F11" s="25">
         <f ca="1">TODAY()-20</f>
-        <v>45530</v>
+        <v>45576</v>
       </c>
       <c r="G11" s="18">
         <v>1</v>
@@ -1908,11 +1937,11 @@
       </c>
       <c r="I11" s="25">
         <f ca="1">TODAY()-44</f>
-        <v>45506</v>
+        <v>45552</v>
       </c>
       <c r="J11" s="25">
         <f ca="1">TODAY()-15</f>
-        <v>45535</v>
+        <v>45581</v>
       </c>
       <c r="K11" s="18">
         <v>5</v>
@@ -1924,7 +1953,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
@@ -1933,42 +1962,42 @@
         <v>3</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="25">
         <f ca="1">TODAY()-39</f>
-        <v>45511</v>
+        <v>45557</v>
       </c>
       <c r="F12" s="25">
         <f ca="1">TODAY()</f>
-        <v>45550</v>
+        <v>45596</v>
       </c>
       <c r="G12" s="18">
         <v>1</v>
       </c>
       <c r="H12" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$E12,'Project tracker'!$F12)&lt;&gt;2,"",DAYS360('Project tracker'!$E12,'Project tracker'!$F12,FALSE))</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I12" s="25">
         <f ca="1">TODAY()-45</f>
-        <v>45505</v>
+        <v>45551</v>
       </c>
       <c r="J12" s="25">
         <f ca="1">TODAY()-5</f>
-        <v>45545</v>
+        <v>45591</v>
       </c>
       <c r="K12" s="18">
         <v>7</v>
       </c>
       <c r="L12" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$I12,'Project tracker'!$J12)&lt;&gt;2,"",DAYS360('Project tracker'!$I12,'Project tracker'!$J12,FALSE))</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M12" s="18"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="18" t="s">
         <v>30</v>
@@ -1977,30 +2006,30 @@
         <v>5</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="25">
         <f ca="1">TODAY()-95</f>
-        <v>45455</v>
+        <v>45501</v>
       </c>
       <c r="F13" s="25">
         <f ca="1">TODAY()-75</f>
-        <v>45475</v>
+        <v>45521</v>
       </c>
       <c r="G13" s="18">
         <v>1</v>
       </c>
       <c r="H13" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$E13,'Project tracker'!$F13)&lt;&gt;2,"",DAYS360('Project tracker'!$E13,'Project tracker'!$F13,FALSE))</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45460</v>
+        <v>45506</v>
       </c>
       <c r="J13" s="25">
         <f ca="1">TODAY()-80</f>
-        <v>45470</v>
+        <v>45516</v>
       </c>
       <c r="K13" s="18">
         <v>7</v>
@@ -2012,7 +2041,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -2076,39 +2105,39 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="20.08984375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="27"/>
+    <col min="1" max="1" width="12.69921875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="20.09765625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="16.69921875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.69921875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>24</v>
       </c>
@@ -2128,24 +2157,24 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" style="12" customWidth="1"/>
-    <col min="2" max="3" width="18.453125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="6.69921875" style="12" customWidth="1"/>
+    <col min="2" max="3" width="18.5" style="23" customWidth="1"/>
+    <col min="4" max="4" width="6.69921875" style="13" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="16" t="s">
         <v>7</v>
@@ -2153,13 +2182,13 @@
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="3" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="1:4" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="22" t="s">
         <v>8</v>
@@ -2169,67 +2198,67 @@
       </c>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="22" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="22" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="22" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="22" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -2251,6 +2280,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2562,36 +2620,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9066C173-72E5-4455-ACFB-9A7596D30A2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648F31BC-5AA3-42BF-80F4-A797E59C4FBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D99023F8-0F96-4650-8DC3-63EE0BD6CB59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2612,26 +2661,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648F31BC-5AA3-42BF-80F4-A797E59C4FBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9066C173-72E5-4455-ACFB-9A7596D30A2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
Update universal project tracker with Game Logic Timeline, Networking Timeline, Authentication Timeline
</commit_message>
<xml_diff>
--- a/Project tracker.xlsx
+++ b/Project tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BDACB8-4CCA-402D-843C-F093367ADDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56375A83-7D3A-4D1F-B8EC-53E3E73892C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Category</t>
   </si>
@@ -44,13 +44,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Category 1</t>
-  </si>
-  <si>
     <t>Category 2</t>
-  </si>
-  <si>
-    <t>Category 3</t>
   </si>
   <si>
     <t>Category 4</t>
@@ -115,12 +109,6 @@
     <t>Task 3</t>
   </si>
   <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
     <t>Task 6</t>
   </si>
   <si>
@@ -139,15 +127,9 @@
     <t>Student 2</t>
   </si>
   <si>
-    <t>Student 3</t>
-  </si>
-  <si>
     <t>Student 5</t>
   </si>
   <si>
-    <t>Student 4</t>
-  </si>
-  <si>
     <t>Student 6</t>
   </si>
   <si>
@@ -194,6 +176,15 @@
   </si>
   <si>
     <t>Game Functionality Testing</t>
+  </si>
+  <si>
+    <t>Authentication Functionality</t>
+  </si>
+  <si>
+    <t>Authentication Functionality Testing</t>
+  </si>
+  <si>
+    <t>Networking Stubs</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1528,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:F23"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1574,13 +1565,13 @@
     <row r="2" spans="1:14" s="5" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="26" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="9">
         <v>0.25</v>
@@ -1612,37 +1603,37 @@
     <row r="4" spans="1:14" s="5" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="G4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="I4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="24" t="s">
+      <c r="K4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>16</v>
       </c>
       <c r="M4" s="17" t="s">
         <v>1</v>
@@ -1652,13 +1643,13 @@
     <row r="5" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E5" s="25">
         <v>45604</v>
@@ -1694,13 +1685,13 @@
     <row r="6" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E6" s="25">
         <v>45619</v>
@@ -1736,28 +1727,26 @@
     <row r="7" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="18" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E7" s="25">
-        <f ca="1">TODAY()-100</f>
-        <v>45496</v>
+        <v>45604</v>
       </c>
       <c r="F7" s="25">
-        <f ca="1">TODAY()-40</f>
-        <v>45556</v>
+        <v>45621</v>
       </c>
       <c r="G7" s="18">
         <v>5</v>
       </c>
       <c r="H7" s="21">
-        <f ca="1">IF(COUNTA('Project tracker'!$E7,'Project tracker'!$F7)&lt;&gt;2,"",DAYS360('Project tracker'!$E7,'Project tracker'!$F7,FALSE))</f>
-        <v>58</v>
+        <f>IF(COUNTA('Project tracker'!$E7,'Project tracker'!$F7)&lt;&gt;2,"",DAYS360('Project tracker'!$E7,'Project tracker'!$F7,FALSE))</f>
+        <v>17</v>
       </c>
       <c r="I7" s="25">
         <f ca="1">TODAY()-100</f>
@@ -1780,28 +1769,26 @@
     <row r="8" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="18" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E8" s="25">
-        <f ca="1">TODAY()-90</f>
-        <v>45506</v>
+        <v>45619</v>
       </c>
       <c r="F8" s="25">
-        <f ca="1">TODAY()-80</f>
-        <v>45516</v>
+        <v>45622</v>
       </c>
       <c r="G8" s="18">
         <v>6</v>
       </c>
       <c r="H8" s="21">
-        <f ca="1">IF(COUNTA('Project tracker'!$E8,'Project tracker'!$F8)&lt;&gt;2,"",DAYS360('Project tracker'!$E8,'Project tracker'!$F8,FALSE))</f>
-        <v>10</v>
+        <f>IF(COUNTA('Project tracker'!$E8,'Project tracker'!$F8)&lt;&gt;2,"",DAYS360('Project tracker'!$E8,'Project tracker'!$F8,FALSE))</f>
+        <v>3</v>
       </c>
       <c r="I8" s="25">
         <f ca="1">TODAY()-90</f>
@@ -1824,28 +1811,26 @@
     <row r="9" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="18" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E9" s="25">
-        <f ca="1">TODAY()-90</f>
-        <v>45506</v>
+        <v>45607</v>
       </c>
       <c r="F9" s="25">
-        <f ca="1">TODAY()-50</f>
-        <v>45546</v>
+        <v>45614</v>
       </c>
       <c r="G9" s="18">
         <v>4</v>
       </c>
       <c r="H9" s="21">
-        <f ca="1">IF(COUNTA('Project tracker'!$E9,'Project tracker'!$F9)&lt;&gt;2,"",DAYS360('Project tracker'!$E9,'Project tracker'!$F9,FALSE))</f>
-        <v>39</v>
+        <f>IF(COUNTA('Project tracker'!$E9,'Project tracker'!$F9)&lt;&gt;2,"",DAYS360('Project tracker'!$E9,'Project tracker'!$F9,FALSE))</f>
+        <v>7</v>
       </c>
       <c r="I9" s="25">
         <f ca="1">TODAY()-90</f>
@@ -1868,13 +1853,13 @@
     <row r="10" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E10" s="25">
         <f ca="1">TODAY()-60</f>
@@ -1912,13 +1897,13 @@
     <row r="11" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>32</v>
       </c>
       <c r="E11" s="25">
         <f ca="1">TODAY()-44</f>
@@ -1956,13 +1941,13 @@
     <row r="12" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E12" s="25">
         <f ca="1">TODAY()-39</f>
@@ -2000,13 +1985,13 @@
     <row r="13" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E13" s="25">
         <f ca="1">TODAY()-95</f>
@@ -2118,28 +2103,28 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2177,7 +2162,7 @@
     <row r="2" spans="1:4" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2191,70 +2176,70 @@
     <row r="4" spans="1:4" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="22" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="22" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D10" s="13"/>
     </row>

</xml_diff>